<commit_message>
Modified Excel sheets for consistency
</commit_message>
<xml_diff>
--- a/test_files/data-samples/test-case-03/Input_4_gene_testing.xlsx
+++ b/test_files/data-samples/test-case-03/Input_4_gene_testing.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="644"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="644" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -14,8 +14,7 @@
     <sheet name="network" sheetId="5" r:id="rId5"/>
     <sheet name="network_weights" sheetId="11" r:id="rId6"/>
     <sheet name="optimization_parameters" sheetId="6" r:id="rId7"/>
-    <sheet name="simulation_times" sheetId="14" r:id="rId8"/>
-    <sheet name="network_b" sheetId="16" r:id="rId9"/>
+    <sheet name="network_b" sheetId="16" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">network!$A$1:$V$22</definedName>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
   <si>
     <t>CIN5</t>
   </si>
@@ -121,13 +120,16 @@
   </si>
   <si>
     <t>dcin5</t>
+  </si>
+  <si>
+    <t>simtime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -253,6 +255,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -331,6 +338,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -365,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,21 +549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -568,7 +577,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -580,7 +589,7 @@
       </c>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -592,7 +601,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -605,7 +614,7 @@
       <c r="E4" s="5"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -618,111 +627,111 @@
       <c r="E5" s="5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="4"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="4"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" s="4"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="4"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="4"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" s="4"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" s="4"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" s="4"/>
       <c r="E13" s="5"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="4"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" s="4"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="4"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" s="4"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="4"/>
       <c r="E19" s="5"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20" s="4"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="H22"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E24" s="5"/>
     </row>
   </sheetData>
@@ -734,14 +743,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
@@ -749,7 +758,7 @@
     <col min="4" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -760,7 +769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -771,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -782,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -793,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -804,87 +813,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -898,16 +907,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -954,7 +963,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1001,7 +1010,7 @@
         <v>-1.2219770014641</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1048,7 +1057,7 @@
         <v>-0.48651707588210702</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>1.55526169350673</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1142,31 +1151,31 @@
         <v>-0.19414868863404999</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G6" s="2"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J10" s="2"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G12" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I14" s="2"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="18" spans="4:13">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
       <c r="I18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="4:13">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="4:13">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
       <c r="F20" s="2"/>
       <c r="M20" s="2"/>
     </row>
@@ -1178,16 +1187,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>-1.2219770014641</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1328,7 +1337,7 @@
         <v>-0.48651707588210702</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>1.55526169350673</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1422,51 +1431,51 @@
         <v>-0.19414868863404999</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L7" s="2"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C15" s="2"/>
     </row>
-    <row r="18" spans="7:14">
+    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="7:14">
+    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
       <c r="I19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="7:14">
+    <row r="20" spans="7:14" x14ac:dyDescent="0.2">
       <c r="I20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="22" spans="7:14">
+    <row r="22" spans="7:14" x14ac:dyDescent="0.2">
       <c r="L22" s="2"/>
       <c r="N22" s="2"/>
     </row>
@@ -1478,14 +1487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.25" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
@@ -1507,7 +1516,7 @@
     <col min="23" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1524,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
@@ -1541,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1558,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1601,14 +1610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37.25" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.125" style="4" bestFit="1" customWidth="1"/>
@@ -1629,7 +1638,7 @@
     <col min="21" max="22" width="5.125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -1663,7 +1672,7 @@
       <c r="U1"/>
       <c r="V1"/>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1680,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1697,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1740,19 +1749,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1780,7 +1789,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +1813,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1812,7 +1821,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1820,7 +1829,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1828,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1836,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1852,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="12.75" customHeight="1">
+    <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1860,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1">
+    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1874,7 +1883,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1885,7 +1894,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1896,7 +1905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1905,6 +1914,74 @@
       </c>
       <c r="C16">
         <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <v>0.2</v>
+      </c>
+      <c r="E17">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F17">
+        <v>0.4</v>
+      </c>
+      <c r="G17">
+        <v>0.5</v>
+      </c>
+      <c r="H17">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="I17">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="J17">
+        <v>0.8</v>
+      </c>
+      <c r="K17">
+        <v>0.9</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N17">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="O17">
+        <v>1.3</v>
+      </c>
+      <c r="P17">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="Q17">
+        <v>1.5</v>
+      </c>
+      <c r="R17">
+        <v>1.6</v>
+      </c>
+      <c r="S17">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="T17">
+        <v>1.8</v>
+      </c>
+      <c r="U17">
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="V17">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1916,105 +1993,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>0.1</v>
-      </c>
-      <c r="D1">
-        <v>0.2</v>
-      </c>
-      <c r="E1">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F1">
-        <v>0.4</v>
-      </c>
-      <c r="G1">
-        <v>0.5</v>
-      </c>
-      <c r="H1">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="I1">
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="J1">
-        <v>0.8</v>
-      </c>
-      <c r="K1">
-        <v>0.9</v>
-      </c>
-      <c r="L1">
-        <v>1</v>
-      </c>
-      <c r="M1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N1">
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="O1">
-        <v>1.3</v>
-      </c>
-      <c r="P1">
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="Q1">
-        <v>1.5</v>
-      </c>
-      <c r="R1">
-        <v>1.6</v>
-      </c>
-      <c r="S1">
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="T1">
-        <v>1.8</v>
-      </c>
-      <c r="U1">
-        <v>1.9000000000000001</v>
-      </c>
-      <c r="V1">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2022,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2030,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2038,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2046,10 +2039,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
     </row>
   </sheetData>

</xml_diff>